<commit_message>
fixed execl document + add average criteria
</commit_message>
<xml_diff>
--- a/src/uploads/excel/criteria.xlsx
+++ b/src/uploads/excel/criteria.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="161">
   <si>
-    <t xml:space="preserve">id_categorie</t>
+    <t xml:space="preserve">id_category</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -606,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:B279"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A254" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B279" activeCellId="0" sqref="B279"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>